<commit_message>
Up to v0.5. minor fixes, update of figures, `styler`
</commit_message>
<xml_diff>
--- a/data/gpr_settings.xlsx
+++ b/data/gpr_settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raphael/Documents/GitHub/GeoPressureTemplate/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADBD16D7-3DA3-1440-B412-717EA2B0145E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E82ECC3-1BB7-3A49-B25A-1ACE056F9CAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4040" yWindow="1900" windowWidth="27740" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1060" yWindow="500" windowWidth="27740" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tracks" sheetId="1" r:id="rId1"/>
@@ -31,17 +31,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
-  <si>
-    <t>Color</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>mass</t>
   </si>
   <si>
-    <t>RingNo</t>
-  </si>
-  <si>
     <t>gdl_id</t>
   </si>
   <si>
@@ -139,6 +133,15 @@
   </si>
   <si>
     <t>low_speed_fix</t>
+  </si>
+  <si>
+    <t>thr_as</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>ringNo</t>
   </si>
 </sst>
 </file>
@@ -699,12 +702,15 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="15">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -787,13 +793,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3E83695E-4F69-0542-A434-9A92AEDC21B8}" name="Table1" displayName="Table1" ref="A1:AH2" totalsRowShown="0">
-  <autoFilter ref="A1:AH2" xr:uid="{3E83695E-4F69-0542-A434-9A92AEDC21B8}"/>
-  <tableColumns count="34">
-    <tableColumn id="3" xr3:uid="{0E08F938-60A9-C640-A060-C64653A1D0F0}" name="gdl_id" dataDxfId="13" dataCellStyle="Normal_Feuil1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3E83695E-4F69-0542-A434-9A92AEDC21B8}" name="Table1" displayName="Table1" ref="A1:AI2" totalsRowShown="0">
+  <autoFilter ref="A1:AI2" xr:uid="{3E83695E-4F69-0542-A434-9A92AEDC21B8}"/>
+  <tableColumns count="35">
+    <tableColumn id="3" xr3:uid="{0E08F938-60A9-C640-A060-C64653A1D0F0}" name="gdl_id" dataDxfId="14" dataCellStyle="Normal_Feuil1"/>
     <tableColumn id="38" xr3:uid="{5F80A124-B607-6D47-A8B2-B6EBC16D0EC2}" name="crop_start"/>
     <tableColumn id="39" xr3:uid="{C4B8ED7B-88BE-D143-A9A5-6213689753CA}" name="crop_end"/>
-    <tableColumn id="6" xr3:uid="{22680B6F-F907-FD43-BF6C-2E3789C9C356}" name="thr_dur" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{22680B6F-F907-FD43-BF6C-2E3789C9C356}" name="thr_dur" dataDxfId="13"/>
     <tableColumn id="43" xr3:uid="{0ACC25F8-5611-FA4F-B49C-6E30F1D95C08}" name="extent_N"/>
     <tableColumn id="44" xr3:uid="{7341665D-D68F-3E48-95CE-8E270ED9FA6A}" name="extent_W"/>
     <tableColumn id="45" xr3:uid="{18F1D038-2D60-FF49-8711-16897DCC1A1A}" name="extent_S"/>
@@ -804,26 +810,27 @@
     <tableColumn id="50" xr3:uid="{98646B4B-4B26-0A4C-A7C3-1140DBCABB7B}" name="prob_map_s"/>
     <tableColumn id="12" xr3:uid="{A646D821-0BC3-7144-9611-00F929630647}" name="prob_map_s_calib"/>
     <tableColumn id="51" xr3:uid="{AD7A8CAB-A777-7C4D-A6A2-601A4074FBB2}" name="prob_map_thr"/>
-    <tableColumn id="42" xr3:uid="{BF18370D-EF9D-424D-B4AE-3A176A692D5A}" name="shift_k" dataDxfId="11"/>
+    <tableColumn id="42" xr3:uid="{BF18370D-EF9D-424D-B4AE-3A176A692D5A}" name="shift_k" dataDxfId="12"/>
     <tableColumn id="11" xr3:uid="{85327B51-BF51-A643-9746-0720CC021C70}" name="kernel_adjust"/>
     <tableColumn id="9" xr3:uid="{0D248294-1CA3-E44D-A900-569DE950BA49}" name="calib_lon"/>
     <tableColumn id="10" xr3:uid="{50C46AB1-CB9A-B84C-B41F-D6DF90BD8412}" name="calib_lat"/>
-    <tableColumn id="19" xr3:uid="{F555DC9A-9393-234D-92AB-138553DAA03D}" name="calib_1_start" dataDxfId="10"/>
-    <tableColumn id="20" xr3:uid="{F0057B32-84F6-0D4E-B0D3-B8591BCF0A33}" name="calib_1_end" dataDxfId="9"/>
-    <tableColumn id="21" xr3:uid="{72C1CC5C-0A2A-3140-9A33-1BAC20CBDE1B}" name="calib_2_start" dataDxfId="8"/>
-    <tableColumn id="22" xr3:uid="{1E9B142A-92EB-D647-BB56-ADFB8F3B1DE9}" name="calib_2_end" dataDxfId="7"/>
-    <tableColumn id="40" xr3:uid="{ABB1AA27-3007-954E-BFD9-D15B5759E520}" name="calib_2_lon" dataDxfId="6"/>
-    <tableColumn id="41" xr3:uid="{5A6DF468-93CA-8E49-B529-24F965EC5A68}" name="calib_2_lat" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{C1C8E7B8-04FB-6241-9466-61A298BC202A}" name="prob_light_w" dataDxfId="4"/>
-    <tableColumn id="1" xr3:uid="{CA9C149A-C070-ED44-9095-795932D8BA41}" name="thr_prob_percentile" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{74B13C9B-EDD7-A24E-A7E5-146255BCE559}" name="thr_gs" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{4C9C4E26-983D-354E-9081-3E245F2F2396}" name="low_speed_fix" dataDxfId="0"/>
-    <tableColumn id="32" xr3:uid="{8FB298A1-7B27-ED49-9E23-106210114304}" name="RingNo" dataDxfId="1"/>
+    <tableColumn id="19" xr3:uid="{F555DC9A-9393-234D-92AB-138553DAA03D}" name="calib_1_start" dataDxfId="11"/>
+    <tableColumn id="20" xr3:uid="{F0057B32-84F6-0D4E-B0D3-B8591BCF0A33}" name="calib_1_end" dataDxfId="10"/>
+    <tableColumn id="21" xr3:uid="{72C1CC5C-0A2A-3140-9A33-1BAC20CBDE1B}" name="calib_2_start" dataDxfId="9"/>
+    <tableColumn id="22" xr3:uid="{1E9B142A-92EB-D647-BB56-ADFB8F3B1DE9}" name="calib_2_end" dataDxfId="8"/>
+    <tableColumn id="40" xr3:uid="{ABB1AA27-3007-954E-BFD9-D15B5759E520}" name="calib_2_lon" dataDxfId="7"/>
+    <tableColumn id="41" xr3:uid="{5A6DF468-93CA-8E49-B529-24F965EC5A68}" name="calib_2_lat" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{C1C8E7B8-04FB-6241-9466-61A298BC202A}" name="prob_light_w" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{CA9C149A-C070-ED44-9095-795932D8BA41}" name="thr_prob_percentile" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{74B13C9B-EDD7-A24E-A7E5-146255BCE559}" name="thr_gs" dataDxfId="3"/>
+    <tableColumn id="13" xr3:uid="{07BAD23C-A227-CE4D-A5DA-81F573B31782}" name="thr_as" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{4C9C4E26-983D-354E-9081-3E245F2F2396}" name="low_speed_fix" dataDxfId="2"/>
+    <tableColumn id="32" xr3:uid="{8FB298A1-7B27-ED49-9E23-106210114304}" name="ringNo" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{437D6807-140D-EC48-A588-9CA0C70671A6}" name="scientific_name"/>
     <tableColumn id="5" xr3:uid="{E0EF373A-0600-B64D-81CD-63E6714931D7}" name="common_name"/>
     <tableColumn id="34" xr3:uid="{AAB4E28F-C2D5-A44D-A5CF-C6EA295E6EC5}" name="mass"/>
     <tableColumn id="33" xr3:uid="{FE34BCA4-242F-3342-9900-5E0B6676722C}" name="wing_span"/>
-    <tableColumn id="27" xr3:uid="{EFA82C59-4775-1545-BF9E-65F94819FAF1}" name="Color"/>
+    <tableColumn id="27" xr3:uid="{EFA82C59-4775-1545-BF9E-65F94819FAF1}" name="color"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1126,10 +1133,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH13"/>
+  <dimension ref="A1:AI13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AA5" sqref="AA5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1141,125 +1148,128 @@
     <col min="20" max="20" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="15.1640625" customWidth="1"/>
     <col min="22" max="22" width="14.1640625" customWidth="1"/>
-    <col min="23" max="28" width="17.33203125" customWidth="1"/>
-    <col min="30" max="30" width="17.33203125" customWidth="1"/>
-    <col min="31" max="31" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="12.5" customWidth="1"/>
-    <col min="38" max="38" width="16.33203125" customWidth="1"/>
-    <col min="44" max="46" width="15.1640625" customWidth="1"/>
-    <col min="47" max="47" width="14.5" customWidth="1"/>
-    <col min="48" max="48" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="29" width="17.33203125" customWidth="1"/>
+    <col min="31" max="31" width="17.33203125" customWidth="1"/>
+    <col min="32" max="32" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.5" customWidth="1"/>
+    <col min="39" max="39" width="16.33203125" customWidth="1"/>
+    <col min="45" max="47" width="15.1640625" customWidth="1"/>
+    <col min="48" max="48" width="14.5" customWidth="1"/>
+    <col min="49" max="49" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:35">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>6</v>
+      </c>
+      <c r="R1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S1" t="s">
+        <v>10</v>
+      </c>
+      <c r="T1" t="s">
+        <v>11</v>
+      </c>
+      <c r="U1" t="s">
+        <v>12</v>
+      </c>
+      <c r="V1" t="s">
+        <v>13</v>
+      </c>
+      <c r="W1" t="s">
+        <v>14</v>
+      </c>
+      <c r="X1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" t="s">
-        <v>34</v>
-      </c>
-      <c r="N1" t="s">
-        <v>26</v>
-      </c>
-      <c r="O1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>8</v>
-      </c>
-      <c r="R1" t="s">
-        <v>9</v>
-      </c>
-      <c r="S1" t="s">
-        <v>12</v>
-      </c>
-      <c r="T1" t="s">
-        <v>13</v>
-      </c>
-      <c r="U1" t="s">
-        <v>14</v>
-      </c>
-      <c r="V1" t="s">
-        <v>15</v>
-      </c>
-      <c r="W1" t="s">
-        <v>16</v>
-      </c>
-      <c r="X1" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y1" t="s">
+      <c r="AG1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35">
+      <c r="A2" t="s">
         <v>27</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>4</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>5</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>6</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:34">
-      <c r="A2" t="s">
-        <v>29</v>
       </c>
       <c r="B2" s="1">
         <v>42906</v>
@@ -1329,17 +1339,20 @@
         <v>120</v>
       </c>
       <c r="AB2" s="4">
+        <v>100</v>
+      </c>
+      <c r="AC2" s="4">
         <v>15</v>
       </c>
-      <c r="AE2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AH2" s="2"/>
+      <c r="AF2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI2" s="2"/>
     </row>
-    <row r="8" spans="1:34">
+    <row r="8" spans="1:35">
       <c r="R8" s="3"/>
     </row>
-    <row r="13" spans="1:34">
+    <row r="13" spans="1:35">
       <c r="H13" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete check + add wind visual
</commit_message>
<xml_diff>
--- a/data/gpr_settings.xlsx
+++ b/data/gpr_settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raphael/Documents/GitHub/GeoPressureTemplate/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E82ECC3-1BB7-3A49-B25A-1ACE056F9CAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4DCE820-43FD-1146-846B-4573CEF9C622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="500" windowWidth="27740" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1220" yWindow="500" windowWidth="27740" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tracks" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>mass</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>ringNo</t>
+  </si>
+  <si>
+    <t>Acrocephalus arundinaceus</t>
   </si>
 </sst>
 </file>
@@ -704,10 +707,10 @@
   </cellStyles>
   <dxfs count="15">
     <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yy"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -823,9 +826,9 @@
     <tableColumn id="2" xr3:uid="{C1C8E7B8-04FB-6241-9466-61A298BC202A}" name="prob_light_w" dataDxfId="5"/>
     <tableColumn id="1" xr3:uid="{CA9C149A-C070-ED44-9095-795932D8BA41}" name="thr_prob_percentile" dataDxfId="4"/>
     <tableColumn id="7" xr3:uid="{74B13C9B-EDD7-A24E-A7E5-146255BCE559}" name="thr_gs" dataDxfId="3"/>
-    <tableColumn id="13" xr3:uid="{07BAD23C-A227-CE4D-A5DA-81F573B31782}" name="thr_as" dataDxfId="0"/>
-    <tableColumn id="8" xr3:uid="{4C9C4E26-983D-354E-9081-3E245F2F2396}" name="low_speed_fix" dataDxfId="2"/>
-    <tableColumn id="32" xr3:uid="{8FB298A1-7B27-ED49-9E23-106210114304}" name="ringNo" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{07BAD23C-A227-CE4D-A5DA-81F573B31782}" name="thr_as" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{4C9C4E26-983D-354E-9081-3E245F2F2396}" name="low_speed_fix" dataDxfId="1"/>
+    <tableColumn id="32" xr3:uid="{8FB298A1-7B27-ED49-9E23-106210114304}" name="ringNo" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{437D6807-140D-EC48-A588-9CA0C70671A6}" name="scientific_name"/>
     <tableColumn id="5" xr3:uid="{E0EF373A-0600-B64D-81CD-63E6714931D7}" name="common_name"/>
     <tableColumn id="34" xr3:uid="{AAB4E28F-C2D5-A44D-A5CF-C6EA295E6EC5}" name="mass"/>
@@ -1135,8 +1138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AA16" sqref="AA16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1344,6 +1347,9 @@
       <c r="AC2" s="4">
         <v>15</v>
       </c>
+      <c r="AE2" t="s">
+        <v>37</v>
+      </c>
       <c r="AF2" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
spelling check + minor + bump version 0.7
</commit_message>
<xml_diff>
--- a/data/gpr_settings.xlsx
+++ b/data/gpr_settings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raphael/Documents/GitHub/GeoPressureTemplate/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4DCE820-43FD-1146-846B-4573CEF9C622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1034BB4-A3BB-6440-AE7C-9731A11AFD60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1220" yWindow="500" windowWidth="27740" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>mass</t>
   </si>
@@ -136,12 +136,6 @@
   </si>
   <si>
     <t>thr_as</t>
-  </si>
-  <si>
-    <t>color</t>
-  </si>
-  <si>
-    <t>ringNo</t>
   </si>
   <si>
     <t>Acrocephalus arundinaceus</t>
@@ -652,10 +646,9 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -705,10 +698,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yy"/>
-    </dxf>
+  <dxfs count="14">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -796,13 +786,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3E83695E-4F69-0542-A434-9A92AEDC21B8}" name="Table1" displayName="Table1" ref="A1:AI2" totalsRowShown="0">
-  <autoFilter ref="A1:AI2" xr:uid="{3E83695E-4F69-0542-A434-9A92AEDC21B8}"/>
-  <tableColumns count="35">
-    <tableColumn id="3" xr3:uid="{0E08F938-60A9-C640-A060-C64653A1D0F0}" name="gdl_id" dataDxfId="14" dataCellStyle="Normal_Feuil1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3E83695E-4F69-0542-A434-9A92AEDC21B8}" name="Table1" displayName="Table1" ref="A1:AG2" totalsRowShown="0">
+  <autoFilter ref="A1:AG2" xr:uid="{3E83695E-4F69-0542-A434-9A92AEDC21B8}"/>
+  <tableColumns count="33">
+    <tableColumn id="3" xr3:uid="{0E08F938-60A9-C640-A060-C64653A1D0F0}" name="gdl_id" dataDxfId="13" dataCellStyle="Normal_Feuil1"/>
     <tableColumn id="38" xr3:uid="{5F80A124-B607-6D47-A8B2-B6EBC16D0EC2}" name="crop_start"/>
     <tableColumn id="39" xr3:uid="{C4B8ED7B-88BE-D143-A9A5-6213689753CA}" name="crop_end"/>
-    <tableColumn id="6" xr3:uid="{22680B6F-F907-FD43-BF6C-2E3789C9C356}" name="thr_dur" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{22680B6F-F907-FD43-BF6C-2E3789C9C356}" name="thr_dur" dataDxfId="12"/>
     <tableColumn id="43" xr3:uid="{0ACC25F8-5611-FA4F-B49C-6E30F1D95C08}" name="extent_N"/>
     <tableColumn id="44" xr3:uid="{7341665D-D68F-3E48-95CE-8E270ED9FA6A}" name="extent_W"/>
     <tableColumn id="45" xr3:uid="{18F1D038-2D60-FF49-8711-16897DCC1A1A}" name="extent_S"/>
@@ -813,27 +803,25 @@
     <tableColumn id="50" xr3:uid="{98646B4B-4B26-0A4C-A7C3-1140DBCABB7B}" name="prob_map_s"/>
     <tableColumn id="12" xr3:uid="{A646D821-0BC3-7144-9611-00F929630647}" name="prob_map_s_calib"/>
     <tableColumn id="51" xr3:uid="{AD7A8CAB-A777-7C4D-A6A2-601A4074FBB2}" name="prob_map_thr"/>
-    <tableColumn id="42" xr3:uid="{BF18370D-EF9D-424D-B4AE-3A176A692D5A}" name="shift_k" dataDxfId="12"/>
+    <tableColumn id="42" xr3:uid="{BF18370D-EF9D-424D-B4AE-3A176A692D5A}" name="shift_k" dataDxfId="11"/>
     <tableColumn id="11" xr3:uid="{85327B51-BF51-A643-9746-0720CC021C70}" name="kernel_adjust"/>
     <tableColumn id="9" xr3:uid="{0D248294-1CA3-E44D-A900-569DE950BA49}" name="calib_lon"/>
     <tableColumn id="10" xr3:uid="{50C46AB1-CB9A-B84C-B41F-D6DF90BD8412}" name="calib_lat"/>
-    <tableColumn id="19" xr3:uid="{F555DC9A-9393-234D-92AB-138553DAA03D}" name="calib_1_start" dataDxfId="11"/>
-    <tableColumn id="20" xr3:uid="{F0057B32-84F6-0D4E-B0D3-B8591BCF0A33}" name="calib_1_end" dataDxfId="10"/>
-    <tableColumn id="21" xr3:uid="{72C1CC5C-0A2A-3140-9A33-1BAC20CBDE1B}" name="calib_2_start" dataDxfId="9"/>
-    <tableColumn id="22" xr3:uid="{1E9B142A-92EB-D647-BB56-ADFB8F3B1DE9}" name="calib_2_end" dataDxfId="8"/>
-    <tableColumn id="40" xr3:uid="{ABB1AA27-3007-954E-BFD9-D15B5759E520}" name="calib_2_lon" dataDxfId="7"/>
-    <tableColumn id="41" xr3:uid="{5A6DF468-93CA-8E49-B529-24F965EC5A68}" name="calib_2_lat" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{C1C8E7B8-04FB-6241-9466-61A298BC202A}" name="prob_light_w" dataDxfId="5"/>
-    <tableColumn id="1" xr3:uid="{CA9C149A-C070-ED44-9095-795932D8BA41}" name="thr_prob_percentile" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{74B13C9B-EDD7-A24E-A7E5-146255BCE559}" name="thr_gs" dataDxfId="3"/>
-    <tableColumn id="13" xr3:uid="{07BAD23C-A227-CE4D-A5DA-81F573B31782}" name="thr_as" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{4C9C4E26-983D-354E-9081-3E245F2F2396}" name="low_speed_fix" dataDxfId="1"/>
-    <tableColumn id="32" xr3:uid="{8FB298A1-7B27-ED49-9E23-106210114304}" name="ringNo" dataDxfId="0"/>
+    <tableColumn id="19" xr3:uid="{F555DC9A-9393-234D-92AB-138553DAA03D}" name="calib_1_start" dataDxfId="10"/>
+    <tableColumn id="20" xr3:uid="{F0057B32-84F6-0D4E-B0D3-B8591BCF0A33}" name="calib_1_end" dataDxfId="9"/>
+    <tableColumn id="21" xr3:uid="{72C1CC5C-0A2A-3140-9A33-1BAC20CBDE1B}" name="calib_2_start" dataDxfId="8"/>
+    <tableColumn id="22" xr3:uid="{1E9B142A-92EB-D647-BB56-ADFB8F3B1DE9}" name="calib_2_end" dataDxfId="7"/>
+    <tableColumn id="40" xr3:uid="{ABB1AA27-3007-954E-BFD9-D15B5759E520}" name="calib_2_lon" dataDxfId="6"/>
+    <tableColumn id="41" xr3:uid="{5A6DF468-93CA-8E49-B529-24F965EC5A68}" name="calib_2_lat" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{C1C8E7B8-04FB-6241-9466-61A298BC202A}" name="prob_light_w" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{CA9C149A-C070-ED44-9095-795932D8BA41}" name="thr_prob_percentile" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{74B13C9B-EDD7-A24E-A7E5-146255BCE559}" name="thr_gs" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{07BAD23C-A227-CE4D-A5DA-81F573B31782}" name="thr_as" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{4C9C4E26-983D-354E-9081-3E245F2F2396}" name="low_speed_fix" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{437D6807-140D-EC48-A588-9CA0C70671A6}" name="scientific_name"/>
     <tableColumn id="5" xr3:uid="{E0EF373A-0600-B64D-81CD-63E6714931D7}" name="common_name"/>
     <tableColumn id="34" xr3:uid="{AAB4E28F-C2D5-A44D-A5CF-C6EA295E6EC5}" name="mass"/>
     <tableColumn id="33" xr3:uid="{FE34BCA4-242F-3342-9900-5E0B6676722C}" name="wing_span"/>
-    <tableColumn id="27" xr3:uid="{EFA82C59-4775-1545-BF9E-65F94819FAF1}" name="color"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1136,10 +1124,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI13"/>
+  <dimension ref="A1:AG13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AA16" sqref="AA16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1151,19 +1139,18 @@
     <col min="20" max="20" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="15.1640625" customWidth="1"/>
     <col min="22" max="22" width="14.1640625" customWidth="1"/>
-    <col min="23" max="29" width="17.33203125" customWidth="1"/>
-    <col min="31" max="31" width="17.33203125" customWidth="1"/>
-    <col min="32" max="32" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.5" customWidth="1"/>
-    <col min="39" max="39" width="16.33203125" customWidth="1"/>
-    <col min="45" max="47" width="15.1640625" customWidth="1"/>
-    <col min="48" max="48" width="14.5" customWidth="1"/>
-    <col min="49" max="49" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="30" width="17.33203125" customWidth="1"/>
+    <col min="31" max="31" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.5" customWidth="1"/>
+    <col min="37" max="37" width="16.33203125" customWidth="1"/>
+    <col min="43" max="45" width="15.1640625" customWidth="1"/>
+    <col min="46" max="46" width="14.5" customWidth="1"/>
+    <col min="47" max="47" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35">
+    <row r="1" spans="1:33">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1252,25 +1239,19 @@
         <v>33</v>
       </c>
       <c r="AD1" t="s">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="AE1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AG1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AH1" t="s">
         <v>4</v>
       </c>
-      <c r="AI1" t="s">
-        <v>35</v>
-      </c>
     </row>
-    <row r="2" spans="1:35">
+    <row r="2" spans="1:33">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -1280,7 +1261,7 @@
       <c r="C2" s="1">
         <v>43222</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>12</v>
       </c>
       <c r="E2">
@@ -1332,34 +1313,33 @@
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
-      <c r="Y2" s="4">
+      <c r="Y2" s="3">
         <v>0.1</v>
       </c>
-      <c r="Z2" s="4">
+      <c r="Z2" s="3">
         <v>0.9</v>
       </c>
-      <c r="AA2" s="4">
+      <c r="AA2" s="3">
         <v>120</v>
       </c>
-      <c r="AB2" s="4">
+      <c r="AB2" s="3">
         <v>100</v>
       </c>
-      <c r="AC2" s="4">
+      <c r="AC2" s="3">
         <v>15</v>
       </c>
+      <c r="AD2" t="s">
+        <v>35</v>
+      </c>
       <c r="AE2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AF2" t="s">
         <v>28</v>
       </c>
-      <c r="AI2" s="2"/>
     </row>
-    <row r="8" spans="1:35">
-      <c r="R8" s="3"/>
+    <row r="8" spans="1:33">
+      <c r="R8" s="2"/>
     </row>
-    <row r="13" spans="1:35">
-      <c r="H13" s="5"/>
+    <row r="13" spans="1:33">
+      <c r="H13" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>

</xml_diff>